<commit_message>
updated notebook and erdri cds source nb
</commit_message>
<xml_diff>
--- a/res/test_data/erdri/erdri_cds.xlsx
+++ b/res/test_data/erdri/erdri_cds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\OneDrive\Documents\dataspell\rarelink_phenopacket_mapper\res\test_data\erdri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52EE303-8159-49A1-B458-FA47D3E56368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF674F0-C317-40CE-A032-8992738B0F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11442" yWindow="0" windowWidth="11676" windowHeight="13758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,21 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>data_type</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>specification</t>
-  </si>
-  <si>
     <t xml:space="preserve">Patient's pseudonym </t>
   </si>
   <si>
@@ -51,9 +36,6 @@
     <t>1. Pseudonym</t>
   </si>
   <si>
-    <t>section</t>
-  </si>
-  <si>
     <t>2. Personal information</t>
   </si>
   <si>
@@ -136,9 +118,6 @@
   </si>
   <si>
     <t>Diagnosis retained by the specialised centre</t>
-  </si>
-  <si>
-    <t>orpha code, alpha code, icd-9, icd-9-cm, icd-10</t>
   </si>
   <si>
     <t>Orpha code (strongly
@@ -154,9 +133,6 @@
 the specialised centre</t>
   </si>
   <si>
-    <t>hgvs code, hgnc code, omim code</t>
-  </si>
-  <si>
     <t>International classification of
 mutations (HGVS) (strongly
 recommended – see link) /
@@ -170,10 +146,34 @@
 defined</t>
   </si>
   <si>
-    <t>hpo code, hgvs code</t>
-  </si>
-  <si>
     <t>Phenotype (HPO), Genotype (HGVS)</t>
+  </si>
+  <si>
+    <t>orpha, alpha, icd-9, icd-9-cm, icd-10</t>
+  </si>
+  <si>
+    <t>hgvs, hgnc, omim</t>
+  </si>
+  <si>
+    <t>hpo, hgvs</t>
+  </si>
+  <si>
+    <t>data_field_name</t>
+  </si>
+  <si>
+    <t>data_model_section</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>data_types</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>comment</t>
   </si>
 </sst>
 </file>
@@ -497,46 +497,47 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.7890625" customWidth="1"/>
+    <col min="1" max="1" width="19.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.20703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -544,196 +545,196 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
       <c r="E9" t="b">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="14.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E12" t="b">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated erdri cds definition
</commit_message>
<xml_diff>
--- a/res/test_data/erdri/erdri_cds.xlsx
+++ b/res/test_data/erdri/erdri_cds.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\OneDrive\Documents\dataspell\rarelink_phenopacket_mapper\res\test_data\erdri\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\OneDrive\Documents\dataspell\phenopacket_mapper\res\test_data\erdri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF674F0-C317-40CE-A032-8992738B0F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3483E8ED-950F-4F76-ACD1-5B10F879C600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11442" yWindow="0" windowWidth="11676" windowHeight="13758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t xml:space="preserve">Patient's pseudonym </t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>Age at which symptoms/signs first appeared</t>
-  </si>
-  <si>
-    <t>string, date</t>
   </si>
   <si>
     <t>Antenatal, At birth, Date (dd/mm/yyyy), Undetermined</t>
@@ -174,6 +171,12 @@
   </si>
   <si>
     <t>comment</t>
+  </si>
+  <si>
+    <t>antenatal, at birth, dd/mm/yyyy, undetermined</t>
+  </si>
+  <si>
+    <t>alive, dead, lost in follow-up, opted-out</t>
   </si>
 </sst>
 </file>
@@ -497,7 +500,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -508,22 +511,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -593,6 +596,9 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
       <c r="E5" t="b">
         <v>1</v>
       </c>
@@ -645,19 +651,19 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
         <v>23</v>
-      </c>
-      <c r="E8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -665,76 +671,79 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
-        <v>27</v>
+      <c r="D9" t="s">
+        <v>46</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>29</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="14.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="D11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
         <v>36</v>
-      </c>
-      <c r="D12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>